<commit_message>
adjust 0.3 to 0.3.1
</commit_message>
<xml_diff>
--- a/multi-languages.xlsx
+++ b/multi-languages.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22810"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="tank_auth" sheetId="3" r:id="rId1"/>
@@ -9133,10 +9133,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Verion:0.3 DEV.COBUB.COM ';</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>$lang['f_version']</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -9149,10 +9145,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>&amp;copy Copyright 2012, Version:0.3 &lt;a href="http://dev.cobub.com"&gt;COBUB SOLUTION&lt;/a&gt;';</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>$lang['f_detail']</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -9161,8 +9153,13 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>&amp;copy Copyright 2012，版本：0.3 &lt;a href="http://dev.cobub.com"&gt;COBUB SOLUTION&lt;/a&gt;';</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>Verion:0.3.1 DEV.COBUB.COM ';</t>
+  </si>
+  <si>
+    <t>&amp;copy Copyright 2012，版本：0.3.1 &lt;a href="http://dev.cobub.com"&gt;COBUB SOLUTION&lt;/a&gt;';</t>
+  </si>
+  <si>
+    <t>&amp;copy Copyright 2012, Version:0.3.1 &lt;a href="http://dev.cobub.com"&gt;COBUB SOLUTION&lt;/a&gt;';</t>
   </si>
 </sst>
 </file>
@@ -9529,7 +9526,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
@@ -11194,8 +11191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H811"/>
   <sheetViews>
-    <sheetView topLeftCell="A66" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -11633,24 +11630,24 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>3018</v>
+        <v>3017</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>3017</v>
+        <v>3022</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>3017</v>
+        <v>3022</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>3022</v>
+        <v>3020</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>3023</v>
+        <v>3021</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>3020</v>
+        <v>3019</v>
       </c>
     </row>
     <row r="39" spans="1:4">
@@ -11658,13 +11655,13 @@
         <v>118</v>
       </c>
       <c r="B39" s="5" t="s">
+        <v>3023</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>3024</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>3021</v>
-      </c>
       <c r="D39" s="4" t="s">
-        <v>3019</v>
+        <v>3018</v>
       </c>
     </row>
     <row r="41" spans="1:4">

</xml_diff>